<commit_message>
Algorithm for 1 shuttle
</commit_message>
<xml_diff>
--- a/Zone Distance_Time Matrix .xlsx
+++ b/Zone Distance_Time Matrix .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivynguyen/Documents/GitHub/GKTW_Transportation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC90A78-4F68-3A48-A57E-57DFC48CD162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA63520A-AF56-5C46-995C-D989E01D05CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="25600" windowHeight="14860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
     <t>Z</t>
   </si>
   <si>
-    <t>Start</t>
+    <t>Zones</t>
   </si>
 </sst>
 </file>
@@ -68,7 +68,6 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -436,6 +435,9 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
       <c r="C2" s="1">
         <v>1.5</v>
       </c>
@@ -465,6 +467,12 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B3" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
       <c r="D3" s="1">
         <v>1.5</v>
       </c>
@@ -491,6 +499,15 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
       <c r="E4" s="1">
         <v>1.5</v>
       </c>
@@ -514,6 +531,18 @@
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
       <c r="F5" s="1">
         <v>1.5</v>
       </c>
@@ -533,6 +562,21 @@
     <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
       </c>
       <c r="G6" s="1">
         <v>2</v>
@@ -551,6 +595,24 @@
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
       <c r="H7" s="1">
         <v>1.5</v>
       </c>
@@ -565,6 +627,27 @@
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B8" s="1">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
       <c r="I8" s="1">
         <v>1.5</v>
       </c>
@@ -576,6 +659,30 @@
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B9" s="1">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1">
+        <v>4</v>
+      </c>
+      <c r="E9" s="1">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1">
+        <v>3</v>
+      </c>
+      <c r="G9" s="1">
+        <v>2</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1</v>
+      </c>
       <c r="J9" s="1">
         <v>3</v>
       </c>
@@ -583,6 +690,33 @@
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="H10" s="1">
+        <v>2</v>
+      </c>
+      <c r="I10" s="1">
+        <v>3</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>